<commit_message>
revisão e inicio do novo modulo 4
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/2.Formatacao/3.Formatacao_condicional.xlsx
+++ b/2.Excel/hands-on/2.Formatacao/3.Formatacao_condicional.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\5.Formatacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\2.Formatacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD6CE0B-30B1-48CB-893A-6FA4A92355B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D139499E-E602-4E66-92CC-A9A36A815169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11196" yWindow="0" windowWidth="12192" windowHeight="13056" firstSheet="3" activeTab="4" xr2:uid="{60DE4CDD-BFE8-488F-B25C-A1E3AA20DCD1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{60DE4CDD-BFE8-488F-B25C-A1E3AA20DCD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Regras_Realce" sheetId="1" r:id="rId1"/>
@@ -235,91 +235,361 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="35">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -645,7 +915,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -668,10 +938,10 @@
       <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="7"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -926,20 +1196,27 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:B17">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+      <formula>"Internacional"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>"Nacional"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
-      <formula>"Internacional"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
-      <formula>100000</formula>
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="greaterThan">
+      <formula>120000</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="between">
+      <formula>30000</formula>
+      <formula>120000</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="lessThan">
+      <formula>30000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D17">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="lessThan">
       <formula>1000000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -952,7 +1229,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -975,10 +1252,10 @@
       <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="7"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1232,8 +1509,8 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="top10" dxfId="3" priority="3" percent="1" rank="25"/>
-    <cfRule type="top10" dxfId="2" priority="2" percent="1" bottom="1" rank="25"/>
+    <cfRule type="top10" dxfId="2" priority="2" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="0" priority="3" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D17">
     <cfRule type="aboveAverage" dxfId="1" priority="1"/>
@@ -1246,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF437162-3E08-4465-9A62-E94A03D4ADED}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1271,10 +1548,10 @@
       <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="7"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1527,6 +1804,18 @@
   <mergeCells count="1">
     <mergeCell ref="G1:H1"/>
   </mergeCells>
+  <conditionalFormatting sqref="C2:C17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D2:D17">
     <cfRule type="dataBar" priority="2">
       <dataBar>
@@ -1539,18 +1828,6 @@
           <x14:id>{A44D49A9-52DB-4F04-9489-760114A6F9BC}</x14:id>
         </ext>
       </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C17">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF00B0F0"/>
-      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1604,10 +1881,10 @@
       <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="7"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1616,7 +1893,7 @@
       <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>35000</v>
       </c>
       <c r="D2" s="5">
@@ -1636,7 +1913,7 @@
       <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>45000</v>
       </c>
       <c r="D3" s="5">
@@ -1656,7 +1933,7 @@
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>135175</v>
       </c>
       <c r="D4" s="5">
@@ -1676,7 +1953,7 @@
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>7418</v>
       </c>
       <c r="D5" s="5">
@@ -1690,7 +1967,7 @@
       <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>71371</v>
       </c>
       <c r="D6" s="5">
@@ -1704,7 +1981,7 @@
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>0</v>
       </c>
       <c r="D7" s="5">
@@ -1718,7 +1995,7 @@
       <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>145414</v>
       </c>
       <c r="D8" s="5">
@@ -1732,7 +2009,7 @@
       <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>28010</v>
       </c>
       <c r="D9" s="5">
@@ -1746,7 +2023,7 @@
       <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>30523</v>
       </c>
       <c r="D10" s="5">
@@ -1760,7 +2037,7 @@
       <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>0</v>
       </c>
       <c r="D11" s="5">
@@ -1774,7 +2051,7 @@
       <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>47498</v>
       </c>
       <c r="D12" s="5">
@@ -1788,7 +2065,7 @@
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>22285</v>
       </c>
       <c r="D13" s="5">
@@ -1802,7 +2079,7 @@
       <c r="B14" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>71711</v>
       </c>
       <c r="D14" s="5">
@@ -1816,7 +2093,7 @@
       <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>25000</v>
       </c>
       <c r="D15" s="5">
@@ -1830,7 +2107,7 @@
       <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>127481</v>
       </c>
       <c r="D16" s="5">
@@ -1844,7 +2121,7 @@
       <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>5000</v>
       </c>
       <c r="D17" s="5">
@@ -1877,8 +2154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39917C7E-6B08-4271-AC0A-A4B1690F96E5}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1901,10 +2178,10 @@
       <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="7"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -2158,7 +2435,7 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:D17">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="34" priority="1">
       <formula>$C2&gt;75000</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>